<commit_message>
✨I can do it！
</commit_message>
<xml_diff>
--- a/src/main/resources/许愿墙.xlsx
+++ b/src/main/resources/许愿墙.xlsx
@@ -1,172 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FUQUANZN\Desktop\get_jobs2\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D38C95F-896E-4C1F-A8A4-5A1437D5DD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcMode="auto"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>你想找什么样的工作？</t>
-  </si>
-  <si>
-    <t>现在的状态是怎样的？</t>
-  </si>
-  <si>
-    <t>AI攻城狮</t>
-  </si>
-  <si>
-    <t>已找到！</t>
-  </si>
-  <si>
-    <t>Java+AI</t>
-  </si>
-  <si>
-    <t>在找</t>
-  </si>
-  <si>
-    <t>AI agent开发</t>
-  </si>
-  <si>
-    <t>Java实习</t>
-  </si>
-  <si>
-    <t>还没开始找</t>
-  </si>
-  <si>
-    <t>系统架构师</t>
-  </si>
-  <si>
-    <t>Go</t>
-  </si>
-  <si>
-    <t>前端攻城狮</t>
-  </si>
-  <si>
-    <t>AI+游戏开发</t>
-  </si>
-  <si>
-    <t>C++实习</t>
-  </si>
-  <si>
-    <t>后端开发</t>
-  </si>
-  <si>
-    <t>正确的路上</t>
-  </si>
-  <si>
-    <t>Java后端开发</t>
-  </si>
-  <si>
-    <t>在找实习的路上</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>找到了，但是通勤太远想跳槽</t>
-  </si>
-  <si>
-    <t>Frontend leader</t>
-  </si>
-  <si>
-    <t>找到了，但是没有work life balance</t>
-  </si>
-  <si>
-    <t>找到了，不满意</t>
-  </si>
-  <si>
-    <t>Java开发</t>
-  </si>
-  <si>
-    <t>再找</t>
-  </si>
-  <si>
-    <t>前端工程师</t>
-  </si>
-  <si>
-    <t>java开发</t>
-  </si>
-  <si>
-    <t>AI+前端工程师</t>
-  </si>
-  <si>
-    <t>C++开发</t>
-  </si>
-  <si>
-    <t>Go后端开发</t>
-  </si>
-  <si>
-    <t>AI+后端工程师</t>
-  </si>
-  <si>
-    <t>linux运维</t>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF34C724"/>
+        <bgColor/>
       </patternFill>
     </fill>
   </fills>
@@ -232,30 +139,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -563,28 +470,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="false" summaryRight="false"/>
   </sheetPr>
-  <dimension ref="A1:T200"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="74"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="4" t="str">
+        <v>你想找什么样的工作？</v>
+      </c>
+      <c r="B1" s="4" t="str">
+        <v>现在的状态是怎样的？</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -605,12 +512,12 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" s="2" t="str">
+        <v>AI攻城狮</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <v>已找到！</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -631,12 +538,12 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+    <row r="3">
+      <c r="A3" s="2" t="str">
+        <v>Java+AI</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -657,12 +564,12 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+    <row r="4">
+      <c r="A4" s="2" t="str">
+        <v>AI agent开发</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -683,12 +590,12 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
+    <row r="5">
+      <c r="A5" s="2" t="str">
+        <v>Java实习</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <v>还没开始找</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -709,12 +616,12 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
+    <row r="6">
+      <c r="A6" s="2" t="str">
+        <v>系统架构师</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -735,12 +642,12 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
+    <row r="7">
+      <c r="A7" s="2" t="str">
+        <v>Go</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -761,12 +668,12 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
+    <row r="8">
+      <c r="A8" s="2" t="str">
+        <v>前端攻城狮</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -787,12 +694,12 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
+    <row r="9">
+      <c r="A9" s="2" t="str">
+        <v>AI+游戏开发</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -813,12 +720,12 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
+    <row r="10">
+      <c r="A10" s="2" t="str">
+        <v>C++实习</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -839,12 +746,12 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
+    <row r="11">
+      <c r="A11" s="2" t="str">
+        <v>后端开发</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <v>正确的路上</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -865,12 +772,12 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
+    <row r="12">
+      <c r="A12" s="2" t="str">
+        <v>Java后端开发</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <v>在找实习的路上</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -891,12 +798,12 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
+    <row r="13">
+      <c r="A13" s="2" t="str">
+        <v>Java</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <v>找到了，但是通勤太远想跳槽</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -917,12 +824,12 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
+    <row r="14">
+      <c r="A14" s="2" t="str">
+        <v>Frontend leader</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <v>找到了，但是没有work life balance</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -943,12 +850,12 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
+    <row r="15">
+      <c r="A15" s="3" t="str">
+        <v>Java</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <v>找到了，不满意</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -969,12 +876,12 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
+    <row r="16">
+      <c r="A16" s="2" t="str">
+        <v>Java开发</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <v>再找</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -995,12 +902,12 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
+    <row r="17">
+      <c r="A17" s="2" t="str">
+        <v>前端工程师</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1021,12 +928,12 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
+    <row r="18">
+      <c r="A18" s="2" t="str">
+        <v>java开发</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1047,12 +954,12 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
+    <row r="19">
+      <c r="A19" s="2" t="str">
+        <v>AI+前端工程师</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <v>还没开始找</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1073,12 +980,12 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
+    <row r="20">
+      <c r="A20" s="2" t="str">
+        <v>C++开发</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1099,12 +1006,12 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
+    <row r="21">
+      <c r="A21" s="2" t="str">
+        <v>Go</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1125,12 +1032,12 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
+    <row r="22">
+      <c r="A22" s="2" t="str">
+        <v>Go后端开发</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1151,12 +1058,12 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>8</v>
+    <row r="23">
+      <c r="A23" s="2" t="str">
+        <v>AI+后端工程师</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <v>还没开始找</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1177,12 +1084,12 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
+    <row r="24">
+      <c r="A24" s="2" t="str">
+        <v>linux运维</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1203,12 +1110,12 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
+    <row r="25">
+      <c r="A25" s="2" t="str">
+        <v>前端工程师</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <v>在找</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1229,12 +1136,12 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
+    <row r="26">
+      <c r="A26" s="2" t="str">
+        <v>前端工程师</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <v>还没开始找</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1255,9 +1162,13 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+    <row r="27">
+      <c r="A27" s="2" t="str">
+        <v>java开发</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <v>在找</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1277,9 +1188,13 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+    <row r="28">
+      <c r="A28" s="2" t="str">
+        <v>AI+嵌入式</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <v>再找</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1299,9 +1214,13 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+    <row r="29">
+      <c r="A29" s="2" t="str">
+        <v>财务主管</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <v>在找</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1321,9 +1240,13 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+    <row r="30">
+      <c r="A30" s="2" t="str">
+        <v>后端开发</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <v>在学习的路上</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1343,9 +1266,13 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31">
+      <c r="A31" s="2" t="str">
+        <v>去年7月用这个项目找到了第一份工作，现在再次回来，希望跳槽找一份AI售前的工作</v>
+      </c>
+      <c r="B31" s="2" t="str">
+        <v>在找</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1365,9 +1292,13 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+    <row r="32">
+      <c r="A32" s="2" t="str">
+        <v>前端工程师</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <v>在找</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1387,9 +1318,13 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+    <row r="33">
+      <c r="A33" s="2" t="str">
+        <v>Java开发</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <v>准备跳槽</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1409,9 +1344,13 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+    <row r="34">
+      <c r="A34" s="2" t="str">
+        <v>Java开发，有完善的晋升制度</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <v>准备跳槽</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1431,9 +1370,13 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+    <row r="35">
+      <c r="A35" s="2" t="str">
+        <v>前端开发</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <v>在找</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1453,7 +1396,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
@@ -1475,7 +1418,7 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
@@ -1497,7 +1440,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
@@ -1519,7 +1462,7 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
@@ -1541,7 +1484,7 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
@@ -1563,7 +1506,7 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
@@ -1585,7 +1528,7 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -1607,7 +1550,7 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
@@ -1629,7 +1572,7 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
@@ -1651,7 +1594,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
@@ -1673,7 +1616,7 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
@@ -1695,7 +1638,7 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
@@ -1717,7 +1660,7 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
@@ -1739,7 +1682,7 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
@@ -1761,7 +1704,7 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
@@ -1783,7 +1726,7 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
@@ -1805,7 +1748,7 @@
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
@@ -1827,7 +1770,7 @@
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
@@ -1849,7 +1792,7 @@
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
@@ -1871,7 +1814,7 @@
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
@@ -1893,7 +1836,7 @@
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
@@ -1915,7 +1858,7 @@
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
@@ -1937,7 +1880,7 @@
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
@@ -1959,7 +1902,7 @@
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
@@ -1981,7 +1924,7 @@
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
@@ -2003,7 +1946,7 @@
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
@@ -2025,7 +1968,7 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="1"/>
@@ -2047,7 +1990,7 @@
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="1"/>
@@ -2069,7 +2012,7 @@
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="1"/>
@@ -2091,7 +2034,7 @@
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="1"/>
@@ -2113,7 +2056,7 @@
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="1"/>
@@ -2135,7 +2078,7 @@
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="1"/>
@@ -2157,7 +2100,7 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="1"/>
@@ -2179,7 +2122,7 @@
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="1"/>
@@ -2201,7 +2144,7 @@
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="1"/>
@@ -2223,7 +2166,7 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="1"/>
@@ -2245,7 +2188,7 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
@@ -2267,7 +2210,7 @@
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="1"/>
@@ -2289,7 +2232,7 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="1"/>
@@ -2311,7 +2254,7 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="1"/>
@@ -2333,7 +2276,7 @@
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="1"/>
@@ -2355,7 +2298,7 @@
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="1"/>
@@ -2377,7 +2320,7 @@
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="1"/>
@@ -2399,7 +2342,7 @@
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="1"/>
@@ -2421,7 +2364,7 @@
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="1"/>
@@ -2443,7 +2386,7 @@
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="1"/>
@@ -2465,7 +2408,7 @@
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="1"/>
@@ -2487,7 +2430,7 @@
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="1"/>
@@ -2509,7 +2452,7 @@
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
@@ -2531,7 +2474,7 @@
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
@@ -2553,7 +2496,7 @@
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
@@ -2575,7 +2518,7 @@
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="1"/>
@@ -2597,7 +2540,7 @@
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="1"/>
@@ -2619,7 +2562,7 @@
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="1"/>
@@ -2641,7 +2584,7 @@
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="1"/>
@@ -2663,7 +2606,7 @@
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
@@ -2685,7 +2628,7 @@
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="1"/>
@@ -2707,7 +2650,7 @@
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
@@ -2729,7 +2672,7 @@
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
@@ -2751,7 +2694,7 @@
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
@@ -2773,7 +2716,7 @@
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
@@ -2795,7 +2738,7 @@
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
@@ -2817,7 +2760,7 @@
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="1"/>
@@ -2839,7 +2782,7 @@
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="1"/>
@@ -2861,7 +2804,7 @@
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="100">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="1"/>
@@ -2883,7 +2826,7 @@
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="101">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -2905,7 +2848,7 @@
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
@@ -2927,7 +2870,7 @@
       <c r="S102" s="1"/>
       <c r="T102" s="1"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="103">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="1"/>
@@ -2949,7 +2892,7 @@
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="1"/>
@@ -2971,7 +2914,7 @@
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1"/>
@@ -2993,7 +2936,7 @@
       <c r="S105" s="1"/>
       <c r="T105" s="1"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1"/>
@@ -3015,7 +2958,7 @@
       <c r="S106" s="1"/>
       <c r="T106" s="1"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1"/>
@@ -3037,7 +2980,7 @@
       <c r="S107" s="1"/>
       <c r="T107" s="1"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="1"/>
@@ -3059,7 +3002,7 @@
       <c r="S108" s="1"/>
       <c r="T108" s="1"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="1"/>
@@ -3081,7 +3024,7 @@
       <c r="S109" s="1"/>
       <c r="T109" s="1"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="1"/>
@@ -3103,7 +3046,7 @@
       <c r="S110" s="1"/>
       <c r="T110" s="1"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="1"/>
@@ -3125,7 +3068,7 @@
       <c r="S111" s="1"/>
       <c r="T111" s="1"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
@@ -3147,7 +3090,7 @@
       <c r="S112" s="1"/>
       <c r="T112" s="1"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="113">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="1"/>
@@ -3169,7 +3112,7 @@
       <c r="S113" s="1"/>
       <c r="T113" s="1"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="114">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="1"/>
@@ -3191,7 +3134,7 @@
       <c r="S114" s="1"/>
       <c r="T114" s="1"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="115">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="1"/>
@@ -3213,7 +3156,7 @@
       <c r="S115" s="1"/>
       <c r="T115" s="1"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="116">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="1"/>
@@ -3235,7 +3178,7 @@
       <c r="S116" s="1"/>
       <c r="T116" s="1"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="117">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="1"/>
@@ -3257,7 +3200,7 @@
       <c r="S117" s="1"/>
       <c r="T117" s="1"/>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="118">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="1"/>
@@ -3279,7 +3222,7 @@
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="119">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="1"/>
@@ -3301,7 +3244,7 @@
       <c r="S119" s="1"/>
       <c r="T119" s="1"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="120">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="1"/>
@@ -3323,7 +3266,7 @@
       <c r="S120" s="1"/>
       <c r="T120" s="1"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="121">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="1"/>
@@ -3345,7 +3288,7 @@
       <c r="S121" s="1"/>
       <c r="T121" s="1"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="122">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="1"/>
@@ -3367,7 +3310,7 @@
       <c r="S122" s="1"/>
       <c r="T122" s="1"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="123">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="1"/>
@@ -3389,7 +3332,7 @@
       <c r="S123" s="1"/>
       <c r="T123" s="1"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="124">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
@@ -3411,7 +3354,7 @@
       <c r="S124" s="1"/>
       <c r="T124" s="1"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="125">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
@@ -3433,7 +3376,7 @@
       <c r="S125" s="1"/>
       <c r="T125" s="1"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="126">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
@@ -3455,7 +3398,7 @@
       <c r="S126" s="1"/>
       <c r="T126" s="1"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="127">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
@@ -3477,7 +3420,7 @@
       <c r="S127" s="1"/>
       <c r="T127" s="1"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="128">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="1"/>
@@ -3499,7 +3442,7 @@
       <c r="S128" s="1"/>
       <c r="T128" s="1"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="129">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="1"/>
@@ -3521,7 +3464,7 @@
       <c r="S129" s="1"/>
       <c r="T129" s="1"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="130">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="1"/>
@@ -3543,7 +3486,7 @@
       <c r="S130" s="1"/>
       <c r="T130" s="1"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="131">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="1"/>
@@ -3565,7 +3508,7 @@
       <c r="S131" s="1"/>
       <c r="T131" s="1"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="132">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="1"/>
@@ -3587,7 +3530,7 @@
       <c r="S132" s="1"/>
       <c r="T132" s="1"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="133">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="1"/>
@@ -3609,7 +3552,7 @@
       <c r="S133" s="1"/>
       <c r="T133" s="1"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="134">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="1"/>
@@ -3631,7 +3574,7 @@
       <c r="S134" s="1"/>
       <c r="T134" s="1"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="135">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="1"/>
@@ -3653,7 +3596,7 @@
       <c r="S135" s="1"/>
       <c r="T135" s="1"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="136">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="1"/>
@@ -3675,7 +3618,7 @@
       <c r="S136" s="1"/>
       <c r="T136" s="1"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="137">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="1"/>
@@ -3697,7 +3640,7 @@
       <c r="S137" s="1"/>
       <c r="T137" s="1"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="138">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="1"/>
@@ -3719,7 +3662,7 @@
       <c r="S138" s="1"/>
       <c r="T138" s="1"/>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="139">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="1"/>
@@ -3741,7 +3684,7 @@
       <c r="S139" s="1"/>
       <c r="T139" s="1"/>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="140">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
@@ -3763,7 +3706,7 @@
       <c r="S140" s="1"/>
       <c r="T140" s="1"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="141">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="1"/>
@@ -3785,7 +3728,7 @@
       <c r="S141" s="1"/>
       <c r="T141" s="1"/>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="142">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="1"/>
@@ -3807,7 +3750,7 @@
       <c r="S142" s="1"/>
       <c r="T142" s="1"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="143">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="1"/>
@@ -3829,7 +3772,7 @@
       <c r="S143" s="1"/>
       <c r="T143" s="1"/>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="144">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="1"/>
@@ -3851,7 +3794,7 @@
       <c r="S144" s="1"/>
       <c r="T144" s="1"/>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="145">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="1"/>
@@ -3873,7 +3816,7 @@
       <c r="S145" s="1"/>
       <c r="T145" s="1"/>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="146">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="1"/>
@@ -3895,7 +3838,7 @@
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="147">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="1"/>
@@ -3917,7 +3860,7 @@
       <c r="S147" s="1"/>
       <c r="T147" s="1"/>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="148">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="1"/>
@@ -3939,7 +3882,7 @@
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="149">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="1"/>
@@ -3961,7 +3904,7 @@
       <c r="S149" s="1"/>
       <c r="T149" s="1"/>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="150">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="1"/>
@@ -3983,7 +3926,7 @@
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="151">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="1"/>
@@ -4005,7 +3948,7 @@
       <c r="S151" s="1"/>
       <c r="T151" s="1"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="152">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="1"/>
@@ -4027,7 +3970,7 @@
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="153">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="1"/>
@@ -4049,7 +3992,7 @@
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="154">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="1"/>
@@ -4071,7 +4014,7 @@
       <c r="S154" s="1"/>
       <c r="T154" s="1"/>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="155">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="1"/>
@@ -4093,7 +4036,7 @@
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="156">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="1"/>
@@ -4115,7 +4058,7 @@
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="157">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="1"/>
@@ -4137,7 +4080,7 @@
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="158">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="1"/>
@@ -4159,7 +4102,7 @@
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="159">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="1"/>
@@ -4181,7 +4124,7 @@
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="160">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="1"/>
@@ -4203,7 +4146,7 @@
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="161">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="1"/>
@@ -4225,7 +4168,7 @@
       <c r="S161" s="1"/>
       <c r="T161" s="1"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="162">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="1"/>
@@ -4247,7 +4190,7 @@
       <c r="S162" s="1"/>
       <c r="T162" s="1"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="163">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="1"/>
@@ -4269,7 +4212,7 @@
       <c r="S163" s="1"/>
       <c r="T163" s="1"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="164">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="1"/>
@@ -4291,7 +4234,7 @@
       <c r="S164" s="1"/>
       <c r="T164" s="1"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="165">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="1"/>
@@ -4313,7 +4256,7 @@
       <c r="S165" s="1"/>
       <c r="T165" s="1"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="166">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="1"/>
@@ -4335,7 +4278,7 @@
       <c r="S166" s="1"/>
       <c r="T166" s="1"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="167">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="1"/>
@@ -4357,7 +4300,7 @@
       <c r="S167" s="1"/>
       <c r="T167" s="1"/>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="168">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="1"/>
@@ -4379,7 +4322,7 @@
       <c r="S168" s="1"/>
       <c r="T168" s="1"/>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="169">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="1"/>
@@ -4401,7 +4344,7 @@
       <c r="S169" s="1"/>
       <c r="T169" s="1"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="170">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="1"/>
@@ -4423,7 +4366,7 @@
       <c r="S170" s="1"/>
       <c r="T170" s="1"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="171">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="1"/>
@@ -4445,7 +4388,7 @@
       <c r="S171" s="1"/>
       <c r="T171" s="1"/>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="172">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="1"/>
@@ -4467,7 +4410,7 @@
       <c r="S172" s="1"/>
       <c r="T172" s="1"/>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="173">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="1"/>
@@ -4489,7 +4432,7 @@
       <c r="S173" s="1"/>
       <c r="T173" s="1"/>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="174">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="1"/>
@@ -4511,7 +4454,7 @@
       <c r="S174" s="1"/>
       <c r="T174" s="1"/>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="175">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="1"/>
@@ -4533,7 +4476,7 @@
       <c r="S175" s="1"/>
       <c r="T175" s="1"/>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="176">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="1"/>
@@ -4555,7 +4498,7 @@
       <c r="S176" s="1"/>
       <c r="T176" s="1"/>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="177">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="1"/>
@@ -4577,7 +4520,7 @@
       <c r="S177" s="1"/>
       <c r="T177" s="1"/>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="178">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="1"/>
@@ -4599,7 +4542,7 @@
       <c r="S178" s="1"/>
       <c r="T178" s="1"/>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="179">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="1"/>
@@ -4621,7 +4564,7 @@
       <c r="S179" s="1"/>
       <c r="T179" s="1"/>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="180">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="1"/>
@@ -4643,7 +4586,7 @@
       <c r="S180" s="1"/>
       <c r="T180" s="1"/>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="181">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="1"/>
@@ -4665,7 +4608,7 @@
       <c r="S181" s="1"/>
       <c r="T181" s="1"/>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="182">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="1"/>
@@ -4687,7 +4630,7 @@
       <c r="S182" s="1"/>
       <c r="T182" s="1"/>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="183">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="1"/>
@@ -4709,7 +4652,7 @@
       <c r="S183" s="1"/>
       <c r="T183" s="1"/>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="184">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="1"/>
@@ -4731,7 +4674,7 @@
       <c r="S184" s="1"/>
       <c r="T184" s="1"/>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="185">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="1"/>
@@ -4753,7 +4696,7 @@
       <c r="S185" s="1"/>
       <c r="T185" s="1"/>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="186">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="1"/>
@@ -4775,7 +4718,7 @@
       <c r="S186" s="1"/>
       <c r="T186" s="1"/>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="187">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="1"/>
@@ -4797,7 +4740,7 @@
       <c r="S187" s="1"/>
       <c r="T187" s="1"/>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="188">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="1"/>
@@ -4819,7 +4762,7 @@
       <c r="S188" s="1"/>
       <c r="T188" s="1"/>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="189">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="1"/>
@@ -4841,7 +4784,7 @@
       <c r="S189" s="1"/>
       <c r="T189" s="1"/>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="190">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="1"/>
@@ -4863,7 +4806,7 @@
       <c r="S190" s="1"/>
       <c r="T190" s="1"/>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="191">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="1"/>
@@ -4885,7 +4828,7 @@
       <c r="S191" s="1"/>
       <c r="T191" s="1"/>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="192">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="1"/>
@@ -4907,7 +4850,7 @@
       <c r="S192" s="1"/>
       <c r="T192" s="1"/>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="193">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="1"/>
@@ -4929,7 +4872,7 @@
       <c r="S193" s="1"/>
       <c r="T193" s="1"/>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="194">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="1"/>
@@ -4951,7 +4894,7 @@
       <c r="S194" s="1"/>
       <c r="T194" s="1"/>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="195">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="1"/>
@@ -4973,7 +4916,7 @@
       <c r="S195" s="1"/>
       <c r="T195" s="1"/>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="196">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="1"/>
@@ -4995,7 +4938,7 @@
       <c r="S196" s="1"/>
       <c r="T196" s="1"/>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="197">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="1"/>
@@ -5017,7 +4960,7 @@
       <c r="S197" s="1"/>
       <c r="T197" s="1"/>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="198">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="1"/>
@@ -5039,7 +4982,7 @@
       <c r="S198" s="1"/>
       <c r="T198" s="1"/>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="199">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="1"/>
@@ -5061,7 +5004,7 @@
       <c r="S199" s="1"/>
       <c r="T199" s="1"/>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="200">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="1"/>
@@ -5084,8 +5027,6 @@
       <c r="T200" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>